<commit_message>
added my data for the xl file
</commit_message>
<xml_diff>
--- a/pa1/pa1_data.xlsx
+++ b/pa1/pa1_data.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="20115" windowHeight="8505"/>
+    <workbookView xWindow="120" yWindow="100" windowWidth="20620" windowHeight="13660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>n</t>
   </si>
@@ -363,15 +368,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -387,8 +392,20 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>16</v>
       </c>
@@ -404,8 +421,20 @@
       <c r="F2">
         <v>0.44118400000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>0.56937800000000005</v>
+      </c>
+      <c r="K2">
+        <v>100</v>
+      </c>
+      <c r="L2">
+        <v>0.65653799999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <f>A2*2</f>
         <v>32</v>
@@ -422,8 +451,20 @@
       <c r="F3">
         <v>0.29308299999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>100</v>
+      </c>
+      <c r="I3">
+        <v>0.47383900000000001</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+      <c r="L3">
+        <v>0.59495699999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4">
         <f t="shared" ref="A4:A12" si="0">A3*2</f>
         <v>64</v>
@@ -440,8 +481,20 @@
       <c r="F4">
         <v>0.223242</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="I4">
+        <v>0.44169799999999998</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <v>0.55699100000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>128</v>
@@ -458,8 +511,20 @@
       <c r="F5">
         <v>0.15369099999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5">
+        <v>0.35144300000000001</v>
+      </c>
+      <c r="K5">
+        <v>100</v>
+      </c>
+      <c r="L5">
+        <v>0.50558999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>256</v>
@@ -476,8 +541,20 @@
       <c r="F6">
         <v>0.107319</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6">
+        <v>0.31283100000000003</v>
+      </c>
+      <c r="K6">
+        <v>100</v>
+      </c>
+      <c r="L6">
+        <v>0.49217899999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>512</v>
@@ -494,8 +571,20 @@
       <c r="F7">
         <v>9.1278999999999999E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>100</v>
+      </c>
+      <c r="I7">
+        <v>0.25738499999999997</v>
+      </c>
+      <c r="K7">
+        <v>100</v>
+      </c>
+      <c r="L7">
+        <v>0.43179699999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>1024</v>
@@ -512,8 +601,20 @@
       <c r="F8">
         <v>5.5066999999999998E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>100</v>
+      </c>
+      <c r="I8">
+        <v>0.21321399999999999</v>
+      </c>
+      <c r="K8">
+        <v>100</v>
+      </c>
+      <c r="L8">
+        <v>0.39039600000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>2048</v>
@@ -530,8 +631,20 @@
       <c r="F9">
         <v>4.0403000000000001E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>100</v>
+      </c>
+      <c r="I9">
+        <v>0.20388300000000001</v>
+      </c>
+      <c r="K9">
+        <v>100</v>
+      </c>
+      <c r="L9">
+        <v>0.36187000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>4096</v>
@@ -548,8 +661,20 @@
       <c r="F10">
         <v>2.6398000000000001E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>50</v>
+      </c>
+      <c r="I10">
+        <v>0.15441820000000001</v>
+      </c>
+      <c r="K10">
+        <v>50</v>
+      </c>
+      <c r="L10">
+        <v>0.31226500000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>8192</v>
@@ -566,8 +691,20 @@
       <c r="F11">
         <v>1.8988000000000001E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>40</v>
+      </c>
+      <c r="I11">
+        <v>0.13318313000000001</v>
+      </c>
+      <c r="K11">
+        <v>40</v>
+      </c>
+      <c r="L11">
+        <v>0.2924215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>16384</v>
@@ -584,8 +721,20 @@
       <c r="F12">
         <v>1.4877E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>30</v>
+      </c>
+      <c r="I12">
+        <v>0.11788282999999999</v>
+      </c>
+      <c r="K12">
+        <v>30</v>
+      </c>
+      <c r="L12">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13">
         <f>A12*2</f>
         <v>32768</v>
@@ -602,17 +751,40 @@
       <c r="F13">
         <v>8.5109999999999995E-3</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <v>9.4900200000000004E-2</v>
+      </c>
+      <c r="K13">
+        <v>6</v>
+      </c>
+      <c r="L13">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="B15">
         <v>0</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -622,9 +794,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -634,8 +811,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added more to writeup and included threshold function in code/xl file
</commit_message>
<xml_diff>
--- a/pa1/pa1_data.xlsx
+++ b/pa1/pa1_data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
   <si>
     <t>n</t>
   </si>
@@ -30,6 +30,18 @@
   </si>
   <si>
     <t>max</t>
+  </si>
+  <si>
+    <t>3/log(n)</t>
+  </si>
+  <si>
+    <t>4/log(n)</t>
+  </si>
+  <si>
+    <t>2/log(n)</t>
+  </si>
+  <si>
+    <t>1/log(n)</t>
   </si>
 </sst>
 </file>
@@ -368,15 +380,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,26 +398,38 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
       <c r="E1" t="s">
         <v>1</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
       <c r="H1" t="s">
         <v>1</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
       </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
       <c r="K1" t="s">
         <v>1</v>
       </c>
       <c r="L1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>16</v>
       </c>
@@ -415,26 +439,42 @@
       <c r="C2">
         <v>0.410221</v>
       </c>
+      <c r="D2">
+        <f>1.8/LOG(A2,2)</f>
+        <v>0.45</v>
+      </c>
       <c r="E2">
         <v>100</v>
       </c>
       <c r="F2">
         <v>0.44118400000000002</v>
       </c>
+      <c r="G2">
+        <f>2/LOG(A2,2)</f>
+        <v>0.5</v>
+      </c>
       <c r="H2">
         <v>100</v>
       </c>
       <c r="I2">
         <v>0.56937800000000005</v>
       </c>
+      <c r="J2">
+        <f>3/LOG(A2,2)</f>
+        <v>0.75</v>
+      </c>
       <c r="K2">
         <v>100</v>
       </c>
       <c r="L2">
         <v>0.65653799999999995</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2">
+        <f>4/LOG(A2,2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3">
         <f>A2*2</f>
         <v>32</v>
@@ -445,28 +485,44 @@
       <c r="C3">
         <v>0.194968</v>
       </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D13" si="0">1.8/LOG(A3,2)</f>
+        <v>0.36</v>
+      </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="F3">
         <v>0.29308299999999998</v>
       </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G13" si="1">2/LOG(A3,2)</f>
+        <v>0.4</v>
+      </c>
       <c r="H3">
         <v>100</v>
       </c>
       <c r="I3">
         <v>0.47383900000000001</v>
       </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J13" si="2">3/LOG(A3,2)</f>
+        <v>0.6</v>
+      </c>
       <c r="K3">
         <v>100</v>
       </c>
       <c r="L3">
         <v>0.59495699999999996</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3">
+        <f t="shared" ref="M3:M13" si="3">4/LOG(A3,2)</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4">
-        <f t="shared" ref="A4:A12" si="0">A3*2</f>
+        <f t="shared" ref="A4:A12" si="4">A3*2</f>
         <v>64</v>
       </c>
       <c r="B4">
@@ -475,28 +531,44 @@
       <c r="C4">
         <v>0.13475400000000001</v>
       </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
       <c r="E4">
         <v>100</v>
       </c>
       <c r="F4">
         <v>0.223242</v>
       </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
       <c r="H4">
         <v>100</v>
       </c>
       <c r="I4">
         <v>0.44169799999999998</v>
       </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
       <c r="K4">
         <v>100</v>
       </c>
       <c r="L4">
         <v>0.55699100000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4">
+        <f t="shared" si="3"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>128</v>
       </c>
       <c r="B5">
@@ -505,28 +577,44 @@
       <c r="C5">
         <v>7.9946000000000003E-2</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.25714285714285717</v>
+      </c>
       <c r="E5">
         <v>100</v>
       </c>
       <c r="F5">
         <v>0.15369099999999999</v>
       </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>0.2857142857142857</v>
+      </c>
       <c r="H5">
         <v>100</v>
       </c>
       <c r="I5">
         <v>0.35144300000000001</v>
       </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>0.42857142857142855</v>
+      </c>
       <c r="K5">
         <v>100</v>
       </c>
       <c r="L5">
         <v>0.50558999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>256</v>
       </c>
       <c r="B6">
@@ -535,28 +623,44 @@
       <c r="C6">
         <v>4.7016000000000002E-2</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.22500000000000001</v>
+      </c>
       <c r="E6">
         <v>100</v>
       </c>
       <c r="F6">
         <v>0.107319</v>
       </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
       <c r="H6">
         <v>100</v>
       </c>
       <c r="I6">
         <v>0.31283100000000003</v>
       </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>0.375</v>
+      </c>
       <c r="K6">
         <v>100</v>
       </c>
       <c r="L6">
         <v>0.49217899999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>512</v>
       </c>
       <c r="B7">
@@ -565,28 +669,44 @@
       <c r="C7">
         <v>1.9706999999999999E-2</v>
       </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="E7">
         <v>100</v>
       </c>
       <c r="F7">
         <v>9.1278999999999999E-2</v>
       </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.22222222222222221</v>
+      </c>
       <c r="H7">
         <v>100</v>
       </c>
       <c r="I7">
         <v>0.25738499999999997</v>
       </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
       <c r="K7">
         <v>100</v>
       </c>
       <c r="L7">
         <v>0.43179699999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1024</v>
       </c>
       <c r="B8">
@@ -595,28 +715,44 @@
       <c r="C8">
         <v>1.1650000000000001E-2</v>
       </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
       <c r="E8">
         <v>100</v>
       </c>
       <c r="F8">
         <v>5.5066999999999998E-2</v>
       </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
       <c r="H8">
         <v>100</v>
       </c>
       <c r="I8">
         <v>0.21321399999999999</v>
       </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
       <c r="K8">
         <v>100</v>
       </c>
       <c r="L8">
         <v>0.39039600000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>2048</v>
       </c>
       <c r="B9">
@@ -625,28 +761,44 @@
       <c r="C9">
         <v>5.3449999999999999E-3</v>
       </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0.16363636363636364</v>
+      </c>
       <c r="E9">
         <v>100</v>
       </c>
       <c r="F9">
         <v>4.0403000000000001E-2</v>
       </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.18181818181818182</v>
+      </c>
       <c r="H9">
         <v>100</v>
       </c>
       <c r="I9">
         <v>0.20388300000000001</v>
       </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>0.27272727272727271</v>
+      </c>
       <c r="K9">
         <v>100</v>
       </c>
       <c r="L9">
         <v>0.36187000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>0.36363636363636365</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>4096</v>
       </c>
       <c r="B10">
@@ -655,28 +807,44 @@
       <c r="C10">
         <v>3.5239999999999998E-3</v>
       </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
       <c r="E10">
         <v>50</v>
       </c>
       <c r="F10">
         <v>2.6398000000000001E-2</v>
       </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
       <c r="H10">
         <v>50</v>
       </c>
       <c r="I10">
         <v>0.15441820000000001</v>
       </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
       <c r="K10">
         <v>50</v>
       </c>
       <c r="L10">
         <v>0.31226500000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>8192</v>
       </c>
       <c r="B11">
@@ -685,28 +853,44 @@
       <c r="C11">
         <v>1.684E-3</v>
       </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.13846153846153847</v>
+      </c>
       <c r="E11">
         <v>40</v>
       </c>
       <c r="F11">
         <v>1.8988000000000001E-2</v>
       </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0.15384615384615385</v>
+      </c>
       <c r="H11">
         <v>40</v>
       </c>
       <c r="I11">
         <v>0.13318313000000001</v>
       </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>0.23076923076923078</v>
+      </c>
       <c r="K11">
         <v>40</v>
       </c>
       <c r="L11">
         <v>0.2924215</v>
       </c>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>0.30769230769230771</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>16384</v>
       </c>
       <c r="B12">
@@ -715,26 +899,42 @@
       <c r="C12">
         <v>8.9499999999999996E-4</v>
       </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.12857142857142859</v>
+      </c>
       <c r="E12">
         <v>20</v>
       </c>
       <c r="F12">
         <v>1.4877E-2</v>
       </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0.14285714285714285</v>
+      </c>
       <c r="H12">
         <v>30</v>
       </c>
       <c r="I12">
         <v>0.11788282999999999</v>
       </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>0.21428571428571427</v>
+      </c>
       <c r="K12">
         <v>30</v>
       </c>
       <c r="L12">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>0.2857142857142857</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13">
         <f>A12*2</f>
         <v>32768</v>
@@ -745,26 +945,42 @@
       <c r="C13">
         <v>3.6499999999999998E-4</v>
       </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.12000000000000001</v>
+      </c>
       <c r="E13">
         <v>10</v>
       </c>
       <c r="F13">
         <v>8.5109999999999995E-3</v>
       </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0.13333333333333333</v>
+      </c>
       <c r="H13">
         <v>10</v>
       </c>
       <c r="I13">
         <v>9.4900200000000004E-2</v>
       </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
       <c r="K13">
         <v>6</v>
       </c>
       <c r="L13">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="B15">
         <v>0</v>
       </c>

</xml_diff>